<commit_message>
Spectroscopy plot style updates and code reformatting
</commit_message>
<xml_diff>
--- a/eval/finestructure_fit.xlsx
+++ b/eval/finestructure_fit.xlsx
@@ -1,59 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>amp</t>
+  </si>
+  <si>
+    <t>cen</t>
+  </si>
+  <si>
+    <t>sig</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>amp_err</t>
+  </si>
+  <si>
+    <t>cen_err</t>
+  </si>
+  <si>
+    <t>sig_err</t>
+  </si>
+  <si>
+    <t>off_err</t>
+  </si>
+  <si>
+    <t>redchi</t>
+  </si>
+  <si>
+    <t>Temperature of atomic sample [K]</t>
+  </si>
+  <si>
+    <t>Temperature error [K]</t>
+  </si>
+  <si>
+    <t>sigma theory thermal gas (293.15 K)</t>
+  </si>
   <si>
     <t>file</t>
-  </si>
-  <si>
-    <t>amp</t>
-  </si>
-  <si>
-    <t>cen</t>
-  </si>
-  <si>
-    <t>sig</t>
-  </si>
-  <si>
-    <t>off</t>
-  </si>
-  <si>
-    <t>amp_err</t>
-  </si>
-  <si>
-    <t>cen_err</t>
-  </si>
-  <si>
-    <t>sig_err</t>
-  </si>
-  <si>
-    <t>off_err</t>
-  </si>
-  <si>
-    <t>redchi</t>
-  </si>
-  <si>
-    <t>Temperature of atomic sample [K]</t>
-  </si>
-  <si>
-    <t>Temperature error [K]</t>
-  </si>
-  <si>
-    <t>sigma theory thermal gas (293.15 K)</t>
   </si>
   <si>
     <t>85f2</t>
@@ -72,22 +71,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -102,26 +105,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -409,98 +421,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="n">
-        <v>-0.2057642242310909</v>
-      </c>
-      <c r="C2" t="n">
-        <v>3.91536394470023</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.2684041509101527</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.619501162172215</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.000207788540905159</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.0001540634074036713</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.0002526055191873454</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.0001322546562129303</v>
-      </c>
-      <c r="J2" t="n">
-        <v>3.776758416359856e-06</v>
-      </c>
-      <c r="K2" t="n">
-        <v>447.8933449453305</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.5961330699425611</v>
-      </c>
-      <c r="M2" t="n">
+      <c r="B2">
+        <v>-0.2057642243120949</v>
+      </c>
+      <c r="C2">
+        <v>3.915363948133394</v>
+      </c>
+      <c r="D2">
+        <v>0.2684041510317705</v>
+      </c>
+      <c r="E2">
+        <v>0.6195011621689961</v>
+      </c>
+      <c r="F2">
+        <v>0.0002077885438832753</v>
+      </c>
+      <c r="G2">
+        <v>0.0001540634064188639</v>
+      </c>
+      <c r="H2">
+        <v>0.0002526055197442582</v>
+      </c>
+      <c r="I2">
+        <v>0.0001322546564379572</v>
+      </c>
+      <c r="J2">
+        <v>3.776758416359814e-06</v>
+      </c>
+      <c r="K2">
+        <v>447.893345351224</v>
+      </c>
+      <c r="L2">
+        <v>0.5961330715269564</v>
+      </c>
+      <c r="M2">
         <v>0.2171435194098927</v>
       </c>
     </row>
@@ -508,40 +514,40 @@
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="n">
-        <v>-0.3770892607085968</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.528472953729948</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.310049530849635</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.6481507944605257</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.005779526415535944</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.0004945159300190096</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.002477929923381065</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.004268699570427048</v>
-      </c>
-      <c r="J3" t="n">
-        <v>4.197150952578482e-05</v>
-      </c>
-      <c r="K3" t="n">
-        <v>597.6562259770054</v>
-      </c>
-      <c r="L3" t="n">
-        <v>6.754984978361183</v>
-      </c>
-      <c r="M3" t="n">
+      <c r="B3">
+        <v>-0.3770892608497931</v>
+      </c>
+      <c r="C3">
+        <v>1.528472956134894</v>
+      </c>
+      <c r="D3">
+        <v>0.3100495310065898</v>
+      </c>
+      <c r="E3">
+        <v>0.6481507944483833</v>
+      </c>
+      <c r="F3">
+        <v>0.005779526283672626</v>
+      </c>
+      <c r="G3">
+        <v>0.0004945159312711823</v>
+      </c>
+      <c r="H3">
+        <v>0.002477929883174616</v>
+      </c>
+      <c r="I3">
+        <v>0.004268699492225836</v>
+      </c>
+      <c r="J3">
+        <v>4.197150952578756e-05</v>
+      </c>
+      <c r="K3">
+        <v>597.6562265821025</v>
+      </c>
+      <c r="L3">
+        <v>6.754984872175543</v>
+      </c>
+      <c r="M3">
         <v>0.2171452350266772</v>
       </c>
     </row>
@@ -549,40 +555,40 @@
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="n">
-        <v>-0.07602280928601662</v>
-      </c>
-      <c r="C4" t="n">
-        <v>6.257553465823499</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.2745326937756041</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.6163453188890842</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.0001142656549208871</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.0002406936893593379</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.0004995681911541656</v>
-      </c>
-      <c r="I4" t="n">
-        <v>7.488961931081775e-05</v>
-      </c>
-      <c r="J4" t="n">
-        <v>9.810360600932663e-07</v>
-      </c>
-      <c r="K4" t="n">
-        <v>479.609120718108</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1.234250005171811</v>
-      </c>
-      <c r="M4" t="n">
+      <c r="B4">
+        <v>-0.07602280935723937</v>
+      </c>
+      <c r="C4">
+        <v>6.257553470281558</v>
+      </c>
+      <c r="D4">
+        <v>0.274532694129587</v>
+      </c>
+      <c r="E4">
+        <v>0.616345318921227</v>
+      </c>
+      <c r="F4">
+        <v>0.0001142656558047979</v>
+      </c>
+      <c r="G4">
+        <v>0.000240693689793291</v>
+      </c>
+      <c r="H4">
+        <v>0.000499568189303925</v>
+      </c>
+      <c r="I4">
+        <v>7.488961949692943e-05</v>
+      </c>
+      <c r="J4">
+        <v>9.810360600933398e-07</v>
+      </c>
+      <c r="K4">
+        <v>479.6091219549257</v>
+      </c>
+      <c r="L4">
+        <v>1.234250002191989</v>
+      </c>
+      <c r="M4">
         <v>0.2146324109562804</v>
       </c>
     </row>
@@ -590,44 +596,44 @@
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="n">
-        <v>-0.1657823063170407</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.424083762251632</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.2914211378957287</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.6205651153997884</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.001112894192055703</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.0009722485918424131</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.001512379696611729</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.0007126312440588615</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3.901115312604504e-05</v>
-      </c>
-      <c r="K5" t="n">
-        <v>540.4131885715879</v>
-      </c>
-      <c r="L5" t="n">
-        <v>3.966255851999196</v>
-      </c>
-      <c r="M5" t="n">
+      <c r="B5">
+        <v>-0.1657823063217707</v>
+      </c>
+      <c r="C5">
+        <v>0.4240837641225139</v>
+      </c>
+      <c r="D5">
+        <v>0.2914211379072097</v>
+      </c>
+      <c r="E5">
+        <v>0.6205651153599652</v>
+      </c>
+      <c r="F5">
+        <v>0.001112894189532326</v>
+      </c>
+      <c r="G5">
+        <v>0.0009722485820981196</v>
+      </c>
+      <c r="H5">
+        <v>0.001512379677315301</v>
+      </c>
+      <c r="I5">
+        <v>0.0007126312448997784</v>
+      </c>
+      <c r="J5">
+        <v>3.901115312604716e-05</v>
+      </c>
+      <c r="K5">
+        <v>540.413188614169</v>
+      </c>
+      <c r="L5">
+        <v>3.966255801550062</v>
+      </c>
+      <c r="M5">
         <v>0.2146362288790145</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>